<commit_message>
feat: reading google spreadsheet with definitions
</commit_message>
<xml_diff>
--- a/data/Definitions.xlsx
+++ b/data/Definitions.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="630" yWindow="615" windowWidth="37095" windowHeight="17310"/>
+    <workbookView xWindow="630" yWindow="615" windowWidth="37095" windowHeight="17310" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Observations" sheetId="2" r:id="rId1"/>
@@ -18,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="322">
   <si>
     <t>name</t>
   </si>
@@ -453,9 +458,6 @@
   </si>
   <si>
     <t>id</t>
-  </si>
-  <si>
-    <t>convert</t>
   </si>
   <si>
     <t>5373</t>
@@ -992,7 +994,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1032,6 +1034,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1076,13 +1081,12 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="SignalsTable" displayName="SignalsTable" ref="A1:E181" totalsRowShown="0">
-  <autoFilter ref="A1:E181"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="SignalsTable" displayName="SignalsTable" ref="A1:D181" totalsRowShown="0">
+  <autoFilter ref="A1:D181"/>
+  <tableColumns count="4">
     <tableColumn id="1" name="observation"/>
     <tableColumn id="2" name="id"/>
     <tableColumn id="3" name="name"/>
-    <tableColumn id="4" name="convert"/>
     <tableColumn id="5" name="description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1090,8 +1094,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="ConvertTable" displayName="ConvertTable" ref="A1:D2" totalsRowShown="0">
-  <autoFilter ref="A1:D2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="ConvertTable" displayName="ConvertTable" ref="A1:D14" totalsRowShown="0">
+  <autoFilter ref="A1:D14"/>
   <tableColumns count="4">
     <tableColumn id="3" name="signal id"/>
     <tableColumn id="4" name="signal name"/>
@@ -1389,7 +1393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
@@ -2443,7 +2447,7 @@
         <v>143</v>
       </c>
       <c r="B1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -2454,10 +2458,10 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2465,10 +2469,10 @@
         <v>91</v>
       </c>
       <c r="B3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C3" t="s">
         <v>314</v>
-      </c>
-      <c r="C3" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2476,10 +2480,10 @@
         <v>93</v>
       </c>
       <c r="B4" t="s">
+        <v>315</v>
+      </c>
+      <c r="C4" t="s">
         <v>316</v>
-      </c>
-      <c r="C4" t="s">
-        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -2510,7 +2514,7 @@
         <v>143</v>
       </c>
       <c r="B1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -2521,10 +2525,10 @@
         <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -2537,10 +2541,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E181"/>
+  <dimension ref="A1:D181"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2548,11 +2552,10 @@
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="100.7109375" customWidth="1"/>
+    <col min="4" max="4" width="100.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>143</v>
       </c>
@@ -2563,1990 +2566,1447 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
       </c>
-      <c r="D9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
       <c r="C10" t="s">
         <v>28</v>
       </c>
-      <c r="D10" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
       <c r="C11" t="s">
         <v>31</v>
       </c>
-      <c r="D11" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
       <c r="C12" t="s">
         <v>33</v>
       </c>
-      <c r="D12" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
       <c r="C13" t="s">
         <v>35</v>
       </c>
-      <c r="D13" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
       <c r="C14" t="s">
         <v>37</v>
       </c>
-      <c r="D14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>146</v>
-      </c>
-      <c r="D15" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>147</v>
-      </c>
-      <c r="D16" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>148</v>
-      </c>
-      <c r="D17" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>149</v>
-      </c>
-      <c r="D18" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>150</v>
-      </c>
-      <c r="D19" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>151</v>
-      </c>
-      <c r="D20" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>152</v>
-      </c>
-      <c r="D21" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>153</v>
-      </c>
-      <c r="D22" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>154</v>
-      </c>
-      <c r="D23" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>155</v>
-      </c>
-      <c r="D24" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>156</v>
-      </c>
-      <c r="D25" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>157</v>
-      </c>
-      <c r="D26" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>158</v>
-      </c>
-      <c r="D27" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>47</v>
       </c>
       <c r="B28" t="s">
-        <v>159</v>
-      </c>
-      <c r="D28" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>47</v>
       </c>
       <c r="B29" t="s">
-        <v>160</v>
-      </c>
-      <c r="D29" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>161</v>
-      </c>
-      <c r="D30" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>48</v>
       </c>
       <c r="B31" t="s">
-        <v>162</v>
-      </c>
-      <c r="D31" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>
       <c r="B32" t="s">
-        <v>163</v>
-      </c>
-      <c r="D32" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>49</v>
       </c>
       <c r="B33" t="s">
-        <v>164</v>
-      </c>
-      <c r="D33" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>50</v>
       </c>
       <c r="B34" t="s">
-        <v>165</v>
-      </c>
-      <c r="D34" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>166</v>
-      </c>
-      <c r="D35" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>167</v>
-      </c>
-      <c r="D36" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>53</v>
       </c>
       <c r="B37" t="s">
-        <v>168</v>
-      </c>
-      <c r="D37" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>54</v>
       </c>
       <c r="B38" t="s">
-        <v>169</v>
-      </c>
-      <c r="D38" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>55</v>
       </c>
       <c r="B39" t="s">
-        <v>170</v>
-      </c>
-      <c r="D39" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>56</v>
       </c>
       <c r="B40" t="s">
-        <v>171</v>
-      </c>
-      <c r="D40" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>57</v>
       </c>
       <c r="B41" t="s">
-        <v>172</v>
-      </c>
-      <c r="D41" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>58</v>
       </c>
       <c r="B42" t="s">
-        <v>173</v>
-      </c>
-      <c r="D42" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>59</v>
       </c>
       <c r="B43" t="s">
-        <v>174</v>
-      </c>
-      <c r="D43" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>60</v>
       </c>
       <c r="B44" t="s">
-        <v>175</v>
-      </c>
-      <c r="D44" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>60</v>
       </c>
       <c r="B45" t="s">
-        <v>176</v>
-      </c>
-      <c r="D45" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>61</v>
       </c>
       <c r="B46" t="s">
-        <v>177</v>
-      </c>
-      <c r="D46" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>62</v>
       </c>
       <c r="B47" t="s">
-        <v>178</v>
-      </c>
-      <c r="D47" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>63</v>
       </c>
       <c r="B48" t="s">
-        <v>179</v>
-      </c>
-      <c r="D48" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>64</v>
       </c>
       <c r="B49" t="s">
-        <v>180</v>
-      </c>
-      <c r="D49" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>65</v>
       </c>
       <c r="B50" t="s">
-        <v>181</v>
-      </c>
-      <c r="D50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>66</v>
       </c>
       <c r="B51" t="s">
-        <v>182</v>
-      </c>
-      <c r="D51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>67</v>
       </c>
       <c r="B52" t="s">
-        <v>183</v>
-      </c>
-      <c r="D52" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>68</v>
       </c>
       <c r="B53" t="s">
-        <v>184</v>
-      </c>
-      <c r="D53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>69</v>
       </c>
       <c r="B54" t="s">
-        <v>185</v>
-      </c>
-      <c r="D54" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>70</v>
       </c>
       <c r="B55" t="s">
-        <v>186</v>
-      </c>
-      <c r="D55" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>71</v>
       </c>
       <c r="B56" t="s">
-        <v>187</v>
-      </c>
-      <c r="D56" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>72</v>
       </c>
       <c r="B57" t="s">
-        <v>188</v>
-      </c>
-      <c r="D57" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>73</v>
       </c>
       <c r="B58" t="s">
-        <v>189</v>
-      </c>
-      <c r="D58" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>74</v>
       </c>
       <c r="B59" t="s">
-        <v>190</v>
-      </c>
-      <c r="D59" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>75</v>
       </c>
       <c r="B60" t="s">
-        <v>191</v>
-      </c>
-      <c r="D60" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>76</v>
       </c>
       <c r="B61" t="s">
-        <v>192</v>
-      </c>
-      <c r="D61" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>77</v>
       </c>
       <c r="B62" t="s">
-        <v>193</v>
-      </c>
-      <c r="D62" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>78</v>
       </c>
       <c r="B63" t="s">
-        <v>194</v>
-      </c>
-      <c r="D63" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>79</v>
       </c>
       <c r="B64" t="s">
-        <v>195</v>
-      </c>
-      <c r="D64" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>80</v>
       </c>
       <c r="B65" t="s">
-        <v>196</v>
-      </c>
-      <c r="D65" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>81</v>
       </c>
       <c r="B66" t="s">
-        <v>197</v>
-      </c>
-      <c r="D66" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>82</v>
       </c>
       <c r="B67" t="s">
-        <v>198</v>
-      </c>
-      <c r="D67" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>83</v>
       </c>
       <c r="B68" t="s">
-        <v>199</v>
-      </c>
-      <c r="D68" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>84</v>
       </c>
       <c r="B69" t="s">
-        <v>200</v>
-      </c>
-      <c r="D69" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>85</v>
       </c>
       <c r="B70" t="s">
-        <v>201</v>
-      </c>
-      <c r="D70" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>85</v>
       </c>
       <c r="B71" t="s">
-        <v>202</v>
-      </c>
-      <c r="D71" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>86</v>
       </c>
       <c r="B72" t="s">
-        <v>203</v>
-      </c>
-      <c r="D72" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>86</v>
       </c>
       <c r="B73" t="s">
-        <v>204</v>
-      </c>
-      <c r="D73" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>87</v>
       </c>
       <c r="B74" t="s">
-        <v>205</v>
-      </c>
-      <c r="D74" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>87</v>
       </c>
       <c r="B75" t="s">
-        <v>206</v>
-      </c>
-      <c r="D75" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>88</v>
       </c>
       <c r="B76" t="s">
-        <v>207</v>
-      </c>
-      <c r="D76" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>88</v>
       </c>
       <c r="B77" t="s">
-        <v>208</v>
-      </c>
-      <c r="D77" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>89</v>
       </c>
       <c r="B78" t="s">
-        <v>209</v>
-      </c>
-      <c r="D78" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>89</v>
       </c>
       <c r="B79" t="s">
-        <v>210</v>
-      </c>
-      <c r="D79" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>90</v>
       </c>
       <c r="B80" t="s">
-        <v>211</v>
-      </c>
-      <c r="D80" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>90</v>
       </c>
       <c r="B81" t="s">
-        <v>212</v>
-      </c>
-      <c r="D81" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>91</v>
       </c>
       <c r="B82" t="s">
-        <v>213</v>
-      </c>
-      <c r="D82" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>91</v>
       </c>
       <c r="B83" t="s">
-        <v>214</v>
-      </c>
-      <c r="D83" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>93</v>
       </c>
       <c r="B84" t="s">
-        <v>215</v>
-      </c>
-      <c r="D84" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>93</v>
       </c>
       <c r="B85" t="s">
-        <v>216</v>
-      </c>
-      <c r="D85" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>94</v>
       </c>
       <c r="B86" t="s">
-        <v>217</v>
-      </c>
-      <c r="D86" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>94</v>
       </c>
       <c r="B87" t="s">
-        <v>218</v>
-      </c>
-      <c r="D87" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>95</v>
       </c>
       <c r="B88" t="s">
-        <v>219</v>
-      </c>
-      <c r="D88" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>95</v>
       </c>
       <c r="B89" t="s">
-        <v>220</v>
-      </c>
-      <c r="D89" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>96</v>
       </c>
       <c r="B90" t="s">
-        <v>221</v>
-      </c>
-      <c r="D90" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>97</v>
       </c>
       <c r="B91" t="s">
-        <v>222</v>
-      </c>
-      <c r="D91" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>97</v>
       </c>
       <c r="B92" t="s">
-        <v>223</v>
-      </c>
-      <c r="D92" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>98</v>
       </c>
       <c r="B93" t="s">
-        <v>224</v>
-      </c>
-      <c r="D93" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>99</v>
       </c>
       <c r="B94" t="s">
-        <v>225</v>
-      </c>
-      <c r="D94" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>99</v>
       </c>
       <c r="B95" t="s">
-        <v>226</v>
-      </c>
-      <c r="D95" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>100</v>
       </c>
       <c r="B96" t="s">
-        <v>227</v>
-      </c>
-      <c r="D96" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>101</v>
       </c>
       <c r="B97" t="s">
-        <v>228</v>
-      </c>
-      <c r="D97" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>102</v>
       </c>
       <c r="B98" t="s">
-        <v>229</v>
-      </c>
-      <c r="D98" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>102</v>
       </c>
       <c r="B99" t="s">
-        <v>230</v>
-      </c>
-      <c r="D99" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>102</v>
       </c>
       <c r="B100" t="s">
-        <v>231</v>
-      </c>
-      <c r="D100" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>103</v>
       </c>
       <c r="B101" t="s">
-        <v>232</v>
-      </c>
-      <c r="D101" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>104</v>
       </c>
       <c r="B102" t="s">
-        <v>233</v>
-      </c>
-      <c r="D102" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>105</v>
       </c>
       <c r="B103" t="s">
-        <v>234</v>
-      </c>
-      <c r="D103" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>106</v>
       </c>
       <c r="B104" t="s">
-        <v>235</v>
-      </c>
-      <c r="D104" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>107</v>
       </c>
       <c r="B105" t="s">
-        <v>236</v>
-      </c>
-      <c r="D105" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>108</v>
       </c>
       <c r="B106" t="s">
-        <v>237</v>
-      </c>
-      <c r="D106" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>109</v>
       </c>
       <c r="B107" t="s">
-        <v>238</v>
-      </c>
-      <c r="D107" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>110</v>
       </c>
       <c r="B108" t="s">
-        <v>239</v>
-      </c>
-      <c r="D108" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>111</v>
       </c>
       <c r="B109" t="s">
-        <v>240</v>
-      </c>
-      <c r="D109" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>111</v>
       </c>
       <c r="B110" t="s">
-        <v>242</v>
-      </c>
-      <c r="D110" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>111</v>
       </c>
       <c r="B111" t="s">
-        <v>243</v>
-      </c>
-      <c r="D111" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>244</v>
-      </c>
-      <c r="D112" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>240</v>
-      </c>
-      <c r="D113" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>242</v>
-      </c>
-      <c r="D114" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>112</v>
       </c>
       <c r="B115" t="s">
-        <v>243</v>
-      </c>
-      <c r="D115" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>112</v>
       </c>
       <c r="B116" t="s">
-        <v>244</v>
-      </c>
-      <c r="D116" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>113</v>
       </c>
       <c r="B117" t="s">
-        <v>245</v>
-      </c>
-      <c r="D117" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>114</v>
       </c>
       <c r="B118" t="s">
-        <v>247</v>
-      </c>
-      <c r="D118" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>115</v>
       </c>
       <c r="B119" t="s">
-        <v>248</v>
-      </c>
-      <c r="D119" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>116</v>
       </c>
       <c r="B120" t="s">
-        <v>249</v>
-      </c>
-      <c r="D120" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>117</v>
       </c>
       <c r="B121" t="s">
-        <v>250</v>
-      </c>
-      <c r="D121" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>117</v>
       </c>
       <c r="B122" t="s">
-        <v>251</v>
-      </c>
-      <c r="D122" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>118</v>
       </c>
       <c r="B123" t="s">
-        <v>252</v>
-      </c>
-      <c r="D123" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>118</v>
       </c>
       <c r="B124" t="s">
-        <v>253</v>
-      </c>
-      <c r="D124" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>118</v>
       </c>
       <c r="B125" t="s">
-        <v>254</v>
-      </c>
-      <c r="D125" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>118</v>
       </c>
       <c r="B126" t="s">
-        <v>255</v>
-      </c>
-      <c r="D126" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>119</v>
       </c>
       <c r="B127" t="s">
-        <v>256</v>
-      </c>
-      <c r="D127" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>119</v>
       </c>
       <c r="B128" t="s">
-        <v>257</v>
-      </c>
-      <c r="D128" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>120</v>
       </c>
       <c r="B129" t="s">
-        <v>258</v>
-      </c>
-      <c r="D129" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>121</v>
       </c>
       <c r="B130" t="s">
-        <v>259</v>
-      </c>
-      <c r="D130" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>122</v>
       </c>
       <c r="B131" t="s">
-        <v>260</v>
-      </c>
-      <c r="D131" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>123</v>
       </c>
       <c r="B132" t="s">
-        <v>261</v>
-      </c>
-      <c r="D132" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>124</v>
       </c>
       <c r="B133" t="s">
-        <v>262</v>
-      </c>
-      <c r="D133" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>125</v>
       </c>
       <c r="B134" t="s">
-        <v>263</v>
-      </c>
-      <c r="D134" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>126</v>
       </c>
       <c r="B135" t="s">
-        <v>264</v>
-      </c>
-      <c r="D135" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>126</v>
       </c>
       <c r="B136" t="s">
-        <v>265</v>
-      </c>
-      <c r="D136" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>126</v>
       </c>
       <c r="B137" t="s">
-        <v>266</v>
-      </c>
-      <c r="D137" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>126</v>
       </c>
       <c r="B138" t="s">
-        <v>267</v>
-      </c>
-      <c r="D138" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>127</v>
       </c>
       <c r="B139" t="s">
-        <v>268</v>
-      </c>
-      <c r="D139" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>127</v>
       </c>
       <c r="B140" t="s">
-        <v>269</v>
-      </c>
-      <c r="D140" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>128</v>
       </c>
       <c r="B141" t="s">
-        <v>270</v>
-      </c>
-      <c r="D141" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>129</v>
       </c>
       <c r="B142" t="s">
-        <v>271</v>
-      </c>
-      <c r="D142" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>130</v>
       </c>
       <c r="B143" t="s">
-        <v>272</v>
-      </c>
-      <c r="D143" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>131</v>
       </c>
       <c r="B144" t="s">
-        <v>273</v>
-      </c>
-      <c r="D144" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>131</v>
       </c>
       <c r="B145" t="s">
-        <v>274</v>
-      </c>
-      <c r="D145" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>131</v>
       </c>
       <c r="B146" t="s">
-        <v>275</v>
-      </c>
-      <c r="D146" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>132</v>
       </c>
       <c r="B147" t="s">
-        <v>276</v>
-      </c>
-      <c r="D147" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>133</v>
       </c>
       <c r="B148" t="s">
-        <v>277</v>
-      </c>
-      <c r="D148" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>134</v>
       </c>
       <c r="B149" t="s">
-        <v>278</v>
-      </c>
-      <c r="D149" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>134</v>
       </c>
       <c r="B150" t="s">
-        <v>280</v>
-      </c>
-      <c r="D150" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>134</v>
       </c>
       <c r="B151" t="s">
-        <v>281</v>
-      </c>
-      <c r="D151" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>134</v>
       </c>
       <c r="B152" t="s">
-        <v>282</v>
-      </c>
-      <c r="D152" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>135</v>
       </c>
       <c r="B153" t="s">
-        <v>278</v>
-      </c>
-      <c r="D153" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>135</v>
       </c>
       <c r="B154" t="s">
-        <v>280</v>
-      </c>
-      <c r="D154" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>135</v>
       </c>
       <c r="B155" t="s">
-        <v>281</v>
-      </c>
-      <c r="D155" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>135</v>
       </c>
       <c r="B156" t="s">
-        <v>282</v>
-      </c>
-      <c r="D156" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>136</v>
       </c>
       <c r="B157" t="s">
-        <v>287</v>
-      </c>
-      <c r="D157" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>136</v>
       </c>
       <c r="B158" t="s">
-        <v>288</v>
-      </c>
-      <c r="D158" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>136</v>
       </c>
       <c r="B159" t="s">
-        <v>289</v>
-      </c>
-      <c r="D159" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>137</v>
       </c>
       <c r="B160" t="s">
-        <v>290</v>
-      </c>
-      <c r="D160" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>137</v>
       </c>
       <c r="B161" t="s">
-        <v>291</v>
-      </c>
-      <c r="D161" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>137</v>
       </c>
       <c r="B162" t="s">
-        <v>292</v>
-      </c>
-      <c r="D162" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>137</v>
       </c>
       <c r="B163" t="s">
-        <v>293</v>
-      </c>
-      <c r="D163" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>137</v>
       </c>
       <c r="B164" t="s">
-        <v>294</v>
-      </c>
-      <c r="D164" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>137</v>
       </c>
       <c r="B165" t="s">
-        <v>295</v>
-      </c>
-      <c r="D165" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>137</v>
       </c>
       <c r="B166" t="s">
-        <v>296</v>
-      </c>
-      <c r="D166" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>137</v>
       </c>
       <c r="B167" t="s">
-        <v>297</v>
-      </c>
-      <c r="D167" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>138</v>
       </c>
       <c r="B168" t="s">
-        <v>298</v>
-      </c>
-      <c r="D168" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>138</v>
       </c>
       <c r="B169" t="s">
-        <v>299</v>
-      </c>
-      <c r="D169" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>138</v>
       </c>
       <c r="B170" t="s">
-        <v>300</v>
-      </c>
-      <c r="D170" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>139</v>
       </c>
       <c r="B171" t="s">
-        <v>301</v>
-      </c>
-      <c r="D171" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>139</v>
       </c>
       <c r="B172" t="s">
-        <v>302</v>
-      </c>
-      <c r="D172" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>139</v>
       </c>
       <c r="B173" t="s">
-        <v>303</v>
-      </c>
-      <c r="D173" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>140</v>
       </c>
       <c r="B174" t="s">
-        <v>304</v>
-      </c>
-      <c r="D174" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>140</v>
       </c>
       <c r="B175" t="s">
-        <v>305</v>
-      </c>
-      <c r="D175" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>140</v>
       </c>
       <c r="B176" t="s">
-        <v>306</v>
-      </c>
-      <c r="D176" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>140</v>
       </c>
       <c r="B177" t="s">
-        <v>307</v>
-      </c>
-      <c r="D177" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>141</v>
       </c>
       <c r="B178" t="s">
-        <v>308</v>
-      </c>
-      <c r="D178" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>141</v>
       </c>
       <c r="B179" t="s">
-        <v>309</v>
-      </c>
-      <c r="D179" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>142</v>
       </c>
       <c r="B180" t="s">
-        <v>310</v>
-      </c>
-      <c r="D180" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>142</v>
       </c>
       <c r="B181" t="s">
-        <v>311</v>
-      </c>
-      <c r="D181" t="s">
-        <v>144</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -4559,10 +4019,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4575,16 +4035,120 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B1" t="s">
         <v>321</v>
       </c>
-      <c r="B1" t="s">
-        <v>322</v>
-      </c>
       <c r="C1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>244</v>
+      </c>
+      <c r="C6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>277</v>
+      </c>
+      <c r="C7" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>279</v>
+      </c>
+      <c r="C8" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>280</v>
+      </c>
+      <c r="C9" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>281</v>
+      </c>
+      <c r="C10" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>277</v>
+      </c>
+      <c r="C11" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>279</v>
+      </c>
+      <c r="C12" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>280</v>
+      </c>
+      <c r="C13" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>281</v>
+      </c>
+      <c r="C14" t="s">
+        <v>285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>